<commit_message>
magnetic order complete 05/06/2023 , multitav version 2.00
</commit_message>
<xml_diff>
--- a/src/assets/Files/exampleLoadVoucher.xlsx
+++ b/src/assets/Files/exampleLoadVoucher.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="19200" windowHeight="6828"/>
+    <workbookView xWindow="612" yWindow="612" windowWidth="12156" windowHeight="4980"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ProductSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -15,6 +15,9 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>מספר תו</t>
+  </si>
   <si>
     <t>שם פרטי</t>
   </si>
@@ -27,38 +30,13 @@
   <si>
     <t>טלפון סלולרי</t>
   </si>
-  <si>
-    <t>מספר כרטיס</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="177"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="177"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,7 +58,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -88,45 +66,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -136,39 +101,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,136 +212,200 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
+                <a:tint val="100000"/>
                 <a:shade val="100000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -385,39 +414,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="1" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>